<commit_message>
perbaikan import dan penambahan template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Testing</t>
   </si>
   <si>
-    <t xml:space="preserve">123456789012345678</t>
+    <t xml:space="preserve">1980031020050110</t>
   </si>
   <si>
     <t xml:space="preserve">Penata / III.c</t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Kepala Bidang</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing@email.com</t>
+    <t xml:space="preserve">testing@email.com</t>
   </si>
   <si>
     <t xml:space="preserve">User</t>
@@ -66,7 +66,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +87,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,11 +153,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,7 +287,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -333,7 +339,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Testing@email.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="testing@email.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>